<commit_message>
Pilot Detect works at 10Mb, needs 373Mhz clock for 20Mb
</commit_message>
<xml_diff>
--- a/stcDemod/PrecisionReqmt.xlsx
+++ b/stcDemod/PrecisionReqmt.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frank.ziegler\Documents\GitHub\stcDemod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Semco\Vivado\BS1000_Demod_vivado2017\stcDemod\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12255" windowHeight="6810"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12252" windowHeight="6816"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -844,25 +844,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="J56" sqref="J56"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
-    <col min="19" max="19" width="16.7109375" customWidth="1"/>
-    <col min="21" max="21" width="12.140625" customWidth="1"/>
-    <col min="25" max="25" width="11.85546875" customWidth="1"/>
-    <col min="30" max="30" width="15.85546875" customWidth="1"/>
-    <col min="31" max="31" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" customWidth="1"/>
+    <col min="19" max="19" width="16.6640625" customWidth="1"/>
+    <col min="21" max="21" width="12.109375" customWidth="1"/>
+    <col min="25" max="25" width="11.88671875" customWidth="1"/>
+    <col min="30" max="30" width="15.88671875" customWidth="1"/>
+    <col min="31" max="31" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>11</v>
       </c>
@@ -891,7 +891,7 @@
         <v>11.99964773652837</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
         <v>4</v>
       </c>
@@ -906,7 +906,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="G3" t="s">
         <v>8</v>
       </c>
@@ -914,7 +914,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="G4" t="s">
         <v>9</v>
       </c>
@@ -923,7 +923,7 @@
         <v>1.5384607315063477</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="L5" t="s">
         <v>0</v>
       </c>
@@ -943,7 +943,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>0</v>
       </c>
@@ -984,7 +984,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>95</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>94291</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>105950</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>107290</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>2047.1458984765495</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>3.91252543126458+7.54098734682056i</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>5</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>44.2745056495512+85.6273061807793i</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>6</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>127.177271752837+246.62012466789i</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>7</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>251.116293753088+488.213002927207i</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>8</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>415.873996315649+810.589955338986i</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>9</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>621.202731439992+1213.87659103652i</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>10</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>865.72545928736+1695.97183682938i</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>11</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>1174.814145138+2307.68799492815i</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
       <c r="R20" s="5">
         <v>8</v>
       </c>
@@ -1843,19 +1843,19 @@
         <v>1176.1637241463+2316.0756633715i</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
       <c r="I21" t="s">
         <v>29</v>
       </c>
       <c r="J21" s="1">
-        <f>140000000*4/3</f>
-        <v>186666666.66666666</v>
+        <f>140000000*4/3/2</f>
+        <v>93333333.333333328</v>
       </c>
       <c r="L21" t="s">
         <v>31</v>
       </c>
       <c r="M21" s="1">
-        <v>10000000</v>
+        <v>20000000</v>
       </c>
       <c r="R21" s="5">
         <v>9</v>
@@ -1897,7 +1897,7 @@
         <v>1189.99426685231+2402.88164660213i</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
       <c r="I22" t="s">
         <v>70</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>1218.21218435848+2581.7539624132i</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
       <c r="I23" t="s">
         <v>72</v>
       </c>
@@ -2003,13 +2003,13 @@
         <v>1260.1123724232+2850.03063721021i</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
       <c r="I24" t="s">
         <v>71</v>
       </c>
       <c r="J24" s="17">
         <f>J22/(M21*1.04)*J21</f>
-        <v>59733.333333333336</v>
+        <v>14933.333333333334</v>
       </c>
       <c r="O24">
         <v>616</v>
@@ -2058,13 +2058,13 @@
         <v>1315.43051513158+3207.81814829367i</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
       <c r="I25" t="s">
         <v>73</v>
       </c>
       <c r="J25" s="17">
         <f>J24-J23</f>
-        <v>46421.333333333336</v>
+        <v>1621.3333333333339</v>
       </c>
       <c r="O25">
         <v>824</v>
@@ -2113,7 +2113,7 @@
         <v>1383.89206241632+3655.15808228501i</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
         <v>49</v>
       </c>
@@ -2128,7 +2128,7 @@
       </c>
       <c r="J26">
         <f>J25/26</f>
-        <v>1785.4358974358975</v>
+        <v>62.358974358974379</v>
       </c>
       <c r="R26" s="5">
         <v>14</v>
@@ -2170,7 +2170,7 @@
         <v>1464.84854562924+4189.62345840941i</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
       <c r="E27">
         <v>8325</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>1566.45244186375+4867.42071575851i</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
       <c r="E28">
         <f>J28</f>
         <v>931</v>
@@ -2281,7 +2281,7 @@
         <v>1565.10284261817+4875.80838094565i</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
       <c r="E29">
         <f>3*E28</f>
         <v>2793</v>
@@ -2335,7 +2335,7 @@
         <v>1551.005838252+4962.57149006514i</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
       <c r="E30">
         <f>J29</f>
         <v>49</v>
@@ -2389,7 +2389,7 @@
         <v>1521.69047921224+5141.26722576236i</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
       <c r="E31">
         <f>J28</f>
         <v>931</v>
@@ -2437,7 +2437,7 @@
         <v>1477.3222630084+5409.14679084878i</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>47</v>
       </c>
@@ -2452,7 +2452,7 @@
       </c>
       <c r="J32" s="1">
         <f>J21/2</f>
-        <v>93333333.333333328</v>
+        <v>46666666.666666664</v>
       </c>
       <c r="R32" s="5">
         <v>20</v>
@@ -2494,7 +2494,7 @@
         <v>1417.61681423686+5766.22837730626i</v>
       </c>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>48</v>
       </c>
@@ -2513,7 +2513,7 @@
       </c>
       <c r="J33" s="14">
         <f>1.04*4*M21</f>
-        <v>41600000</v>
+        <v>83200000</v>
       </c>
       <c r="R33" s="5">
         <v>21</v>
@@ -2555,10 +2555,10 @@
         <v>1342.3003949308+6212.46535132669i</v>
       </c>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.3">
       <c r="E34" s="12">
         <f>J24</f>
-        <v>59733.333333333336</v>
+        <v>14933.333333333334</v>
       </c>
       <c r="F34" t="s">
         <v>30</v>
@@ -2568,7 +2568,7 @@
       </c>
       <c r="J34" s="1">
         <f>J32/2</f>
-        <v>46666666.666666664</v>
+        <v>23333333.333333332</v>
       </c>
       <c r="R34" s="5">
         <v>22</v>
@@ -2610,13 +2610,13 @@
         <v>1251.51856661699+6745.34981356781i</v>
       </c>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.3">
       <c r="I35" t="s">
         <v>44</v>
       </c>
       <c r="J35" s="15">
         <f>J33/J34</f>
-        <v>0.89142857142857146</v>
+        <v>3.5657142857142858</v>
       </c>
       <c r="R35" s="5">
         <v>23</v>
@@ -2658,7 +2658,7 @@
         <v>1135.38137499226+7420.80864023419i</v>
       </c>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.3">
       <c r="R36" s="5">
         <v>24</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>1131.46883136654+7428.34961814107i</v>
       </c>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A37" s="22"/>
       <c r="B37" s="22"/>
       <c r="C37" s="22"/>
@@ -2760,7 +2760,7 @@
         <v>1090.86728717961+7506.31164252356i</v>
       </c>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
       <c r="C38" s="21" t="s">
@@ -2774,7 +2774,7 @@
       </c>
       <c r="J38" s="16">
         <f>J24/3208*4-16</f>
-        <v>58.480465502909396</v>
+        <v>2.6201163757273491</v>
       </c>
       <c r="K38" s="16"/>
       <c r="L38" s="13"/>
@@ -2822,7 +2822,7 @@
         <v>1006.97785962194+7666.79254536264i</v>
       </c>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
         <v>51</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>880.81994198246+7907.23418031148i</v>
       </c>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
         <v>54</v>
       </c>
@@ -2923,7 +2923,7 @@
         <v>712.117805344278+8227.56461766284i</v>
       </c>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
         <v>50</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>500.626156031675+8627.6537105797i</v>
       </c>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
         <v>52</v>
       </c>
@@ -3040,7 +3040,7 @@
         <v>247.269892191444+9105.16579840881i</v>
       </c>
     </row>
-    <row r="43" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C43" t="s">
         <v>57</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>-74.885040860312+9710.10271488062i</v>
       </c>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.3">
       <c r="C44" t="s">
         <v>58</v>
       </c>
@@ -3131,7 +3131,7 @@
       <c r="V44" s="6"/>
       <c r="W44" s="6"/>
     </row>
-    <row r="45" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C45" t="s">
         <v>8</v>
       </c>
@@ -3161,7 +3161,7 @@
       </c>
       <c r="R45" s="21"/>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.3">
       <c r="L46" t="s">
         <v>81</v>
       </c>
@@ -3182,7 +3182,7 @@
       </c>
       <c r="AJ46" s="22"/>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.3">
       <c r="C47" s="22" t="s">
         <v>56</v>
       </c>
@@ -3212,7 +3212,7 @@
       <c r="Q47" s="21"/>
       <c r="R47" s="21"/>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.3">
       <c r="C48" t="s">
         <v>68</v>
       </c>
@@ -3227,11 +3227,11 @@
         <v>5</v>
       </c>
       <c r="G48">
-        <f t="shared" ref="G48:G55" si="19">F48-17</f>
+        <f t="shared" ref="G48:G54" si="19">F48-17</f>
         <v>-12</v>
       </c>
       <c r="I48">
-        <f t="shared" ref="I48:I55" si="20">D48*2^-F48</f>
+        <f t="shared" ref="I48:I54" si="20">D48*2^-F48</f>
         <v>0.61538461538461542</v>
       </c>
       <c r="J48" t="str">
@@ -3250,7 +3250,7 @@
       <c r="Q48" s="21"/>
       <c r="R48" s="21"/>
     </row>
-    <row r="49" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C49" t="s">
         <v>59</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>0.40329846153846155</v>
       </c>
       <c r="J49" t="str">
-        <f t="shared" ref="J49:J55" si="21">DEC2HEX(D49*2^-G49,5)</f>
+        <f t="shared" ref="J49:J54" si="21">DEC2HEX(D49*2^-G49,5)</f>
         <v>0CE7D</v>
       </c>
       <c r="L49" t="s">
@@ -3285,7 +3285,7 @@
       <c r="Q49" s="21"/>
       <c r="R49" s="21"/>
     </row>
-    <row r="50" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C50" t="s">
         <v>60</v>
       </c>
@@ -3318,7 +3318,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C51" t="s">
         <v>63</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C52" t="s">
         <v>64</v>
       </c>
@@ -3384,7 +3384,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C53" t="s">
         <v>66</v>
       </c>
@@ -3417,7 +3417,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C54" t="s">
         <v>67</v>
       </c>
@@ -3450,13 +3450,13 @@
         <v>220</v>
       </c>
     </row>
-    <row r="55" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
         <v>115</v>
       </c>
       <c r="D55" s="14">
         <f>D40/J34</f>
-        <v>0.89142857142857146</v>
+        <v>1.7828571428571429</v>
       </c>
       <c r="F55">
         <v>-1</v>
@@ -3466,19 +3466,19 @@
       </c>
       <c r="I55" s="14">
         <f>D55</f>
-        <v>0.89142857142857146</v>
-      </c>
-      <c r="J55" t="str">
+        <v>1.7828571428571429</v>
+      </c>
+      <c r="J55" t="e">
         <f>DEC2HEX(D55*2^-G55,8)</f>
-        <v>E434A9B1</v>
-      </c>
-    </row>
-    <row r="56" spans="3:18" x14ac:dyDescent="0.25">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="56" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C56" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="57" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:18" x14ac:dyDescent="0.3">
       <c r="M57" s="18" t="s">
         <v>84</v>
       </c>
@@ -3486,7 +3486,7 @@
       <c r="O57" s="18"/>
       <c r="P57" s="18"/>
     </row>
-    <row r="58" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D58" t="s">
         <v>104</v>
       </c>
@@ -3502,7 +3502,7 @@
       </c>
       <c r="P58" s="18"/>
     </row>
-    <row r="59" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
         <v>103</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="60" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C60">
         <v>600</v>
       </c>
@@ -3582,7 +3582,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="61" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D61">
         <v>36</v>
       </c>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="P61" s="19"/>
     </row>
-    <row r="62" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D62">
         <v>36</v>
       </c>
@@ -3636,7 +3636,7 @@
       </c>
       <c r="P62" s="19"/>
     </row>
-    <row r="63" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D63">
         <v>36</v>
       </c>
@@ -3654,7 +3654,7 @@
       <c r="O63" s="19"/>
       <c r="P63" s="19"/>
     </row>
-    <row r="64" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D64" t="s">
         <v>105</v>
       </c>
@@ -3667,14 +3667,14 @@
       <c r="O64" s="20"/>
       <c r="P64" s="20"/>
     </row>
-    <row r="65" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:16" x14ac:dyDescent="0.3">
       <c r="L65" s="20"/>
       <c r="M65" s="20"/>
       <c r="N65" s="20"/>
       <c r="O65" s="20"/>
       <c r="P65" s="20"/>
     </row>
-    <row r="66" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D66" t="s">
         <v>104</v>
       </c>
@@ -3684,14 +3684,14 @@
       <c r="O66" s="20"/>
       <c r="P66" s="20"/>
     </row>
-    <row r="67" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:16" x14ac:dyDescent="0.3">
       <c r="L67" s="20"/>
       <c r="M67" s="20"/>
       <c r="N67" s="20"/>
       <c r="O67" s="20"/>
       <c r="P67" s="20"/>
     </row>
-    <row r="68" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D68" t="s">
         <v>108</v>
       </c>
@@ -3701,7 +3701,7 @@
       <c r="O68" s="20"/>
       <c r="P68" s="20"/>
     </row>
-    <row r="69" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C69" t="s">
         <v>96</v>
       </c>
@@ -3723,7 +3723,7 @@
       <c r="O69" s="20"/>
       <c r="P69" s="20"/>
     </row>
-    <row r="70" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C70">
         <f>D69*20</f>
         <v>1920</v>
@@ -3741,7 +3741,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="71" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D71">
         <v>96</v>
       </c>
@@ -3755,7 +3755,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="72" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D72">
         <v>96</v>
       </c>
@@ -3769,7 +3769,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="73" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D73">
         <v>96</v>
       </c>

</xml_diff>

<commit_message>
pilotDetector is functional without FM trellis Detector is functional with Larry's testStcDemod after modification on my end Just need to glue the two together.
</commit_message>
<xml_diff>
--- a/stcDemod/PrecisionReqmt.xlsx
+++ b/stcDemod/PrecisionReqmt.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Semco\Vivado\BS1000_Demod_vivado2017\stcDemod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Semco\Vivado\Demods\stcDemod\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -844,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1848,8 +1848,8 @@
         <v>29</v>
       </c>
       <c r="J21" s="1">
-        <f>140000000*4/3/2</f>
-        <v>93333333.333333328</v>
+        <f>140000000*4/3</f>
+        <v>186666666.66666666</v>
       </c>
       <c r="L21" t="s">
         <v>31</v>
@@ -2009,7 +2009,7 @@
       </c>
       <c r="J24" s="17">
         <f>J22/(M21*1.04)*J21</f>
-        <v>14933.333333333334</v>
+        <v>29866.666666666668</v>
       </c>
       <c r="O24">
         <v>616</v>
@@ -2064,7 +2064,7 @@
       </c>
       <c r="J25" s="17">
         <f>J24-J23</f>
-        <v>1621.3333333333339</v>
+        <v>16554.666666666668</v>
       </c>
       <c r="O25">
         <v>824</v>
@@ -2128,7 +2128,7 @@
       </c>
       <c r="J26">
         <f>J25/26</f>
-        <v>62.358974358974379</v>
+        <v>636.71794871794873</v>
       </c>
       <c r="R26" s="5">
         <v>14</v>
@@ -2452,7 +2452,7 @@
       </c>
       <c r="J32" s="1">
         <f>J21/2</f>
-        <v>46666666.666666664</v>
+        <v>93333333.333333328</v>
       </c>
       <c r="R32" s="5">
         <v>20</v>
@@ -2558,7 +2558,7 @@
     <row r="34" spans="1:36" x14ac:dyDescent="0.3">
       <c r="E34" s="12">
         <f>J24</f>
-        <v>14933.333333333334</v>
+        <v>29866.666666666668</v>
       </c>
       <c r="F34" t="s">
         <v>30</v>
@@ -2568,7 +2568,7 @@
       </c>
       <c r="J34" s="1">
         <f>J32/2</f>
-        <v>23333333.333333332</v>
+        <v>46666666.666666664</v>
       </c>
       <c r="R34" s="5">
         <v>22</v>
@@ -2616,7 +2616,7 @@
       </c>
       <c r="J35" s="15">
         <f>J33/J34</f>
-        <v>3.5657142857142858</v>
+        <v>1.7828571428571429</v>
       </c>
       <c r="R35" s="5">
         <v>23</v>
@@ -2774,7 +2774,7 @@
       </c>
       <c r="J38" s="16">
         <f>J24/3208*4-16</f>
-        <v>2.6201163757273491</v>
+        <v>21.240232751454698</v>
       </c>
       <c r="K38" s="16"/>
       <c r="L38" s="13"/>
@@ -3456,7 +3456,7 @@
       </c>
       <c r="D55" s="14">
         <f>D40/J34</f>
-        <v>1.7828571428571429</v>
+        <v>0.89142857142857146</v>
       </c>
       <c r="F55">
         <v>-1</v>
@@ -3466,11 +3466,11 @@
       </c>
       <c r="I55" s="14">
         <f>D55</f>
-        <v>1.7828571428571429</v>
-      </c>
-      <c r="J55" t="e">
+        <v>0.89142857142857146</v>
+      </c>
+      <c r="J55" t="str">
         <f>DEC2HEX(D55*2^-G55,8)</f>
-        <v>#NUM!</v>
+        <v>E434A9B1</v>
       </c>
     </row>
     <row r="56" spans="3:18" x14ac:dyDescent="0.3">

</xml_diff>